<commit_message>
git merging initial seeds for agents
</commit_message>
<xml_diff>
--- a/data/relationships/agent_size.xlsx
+++ b/data/relationships/agent_size.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanda\Work\spatial_computing\data\relationships\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F57F6A4-8E69-496E-BCBB-ABDFF9412122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA5018A-1004-4C31-8E66-57740C5AB59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>space_name</t>
   </si>
@@ -78,12 +78,6 @@
     <t>workshop</t>
   </si>
   <si>
-    <t>car_park</t>
-  </si>
-  <si>
-    <t>bike_park</t>
-  </si>
-  <si>
     <t>shops</t>
   </si>
   <si>
@@ -97,9 +91,6 @@
   </si>
   <si>
     <t>restaurant</t>
-  </si>
-  <si>
-    <t>vegetation</t>
   </si>
   <si>
     <t>lobby</t>
@@ -667,13 +658,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -965,7 +959,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="9">
-        <v>2100</v>
+        <v>1020</v>
       </c>
       <c r="C16" s="9">
         <v>2</v>
@@ -984,7 +978,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="9">
-        <v>460</v>
+        <v>256</v>
       </c>
       <c r="C17" s="9">
         <v>2</v>
@@ -1003,7 +997,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="9">
-        <v>1020</v>
+        <v>306</v>
       </c>
       <c r="C18" s="9">
         <v>2</v>
@@ -1022,7 +1016,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="9">
-        <v>256</v>
+        <v>10</v>
       </c>
       <c r="C19" s="9">
         <v>2</v>
@@ -1041,7 +1035,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="9">
-        <v>306</v>
+        <v>714</v>
       </c>
       <c r="C20" s="9">
         <v>2</v>
@@ -1060,7 +1054,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="9">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C21" s="9">
         <v>2</v>
@@ -1079,7 +1073,7 @@
         <v>23</v>
       </c>
       <c r="B22" s="9">
-        <v>714</v>
+        <v>510</v>
       </c>
       <c r="C22" s="9">
         <v>2</v>
@@ -1093,81 +1087,24 @@
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="9">
-        <v>6122</v>
-      </c>
-      <c r="C23" s="9">
-        <v>2</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="9">
-        <v>16</v>
-      </c>
-      <c r="C24" s="9">
-        <v>2</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="9">
-        <v>510</v>
-      </c>
-      <c r="C25" s="9">
-        <v>2</v>
-      </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-    </row>
-    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="12">
+      <c r="B23" s="12">
         <v>204</v>
       </c>
-      <c r="C26" s="12">
-        <v>2</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
+      <c r="C23" s="12">
+        <v>2</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
merging co-cooking with the spaces
</commit_message>
<xml_diff>
--- a/data/relationships/agent_size.xlsx
+++ b/data/relationships/agent_size.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanda\Work\spatial_computing\data\relationships\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA5018A-1004-4C31-8E66-57740C5AB59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CD3851-B043-4D1C-9C44-81835FCEED95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>space_name</t>
   </si>
@@ -39,21 +39,12 @@
     <t>student_housing</t>
   </si>
   <si>
-    <t>co_cooking_A</t>
-  </si>
-  <si>
     <t>assisted_living</t>
   </si>
   <si>
-    <t>co_cooking_B</t>
-  </si>
-  <si>
     <t>starter_housing</t>
   </si>
   <si>
-    <t>co_cooking_C</t>
-  </si>
-  <si>
     <t>co_working</t>
   </si>
   <si>
@@ -100,6 +91,9 @@
   </si>
   <si>
     <t>arcade</t>
+  </si>
+  <si>
+    <t>voxel_depth</t>
   </si>
 </sst>
 </file>
@@ -658,15 +652,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -679,7 +676,9 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -693,12 +692,14 @@
         <v>3</v>
       </c>
       <c r="B2" s="6">
-        <v>1632</v>
+        <v>1879</v>
       </c>
       <c r="C2" s="6">
         <v>2</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="5">
+        <v>13</v>
+      </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -712,7 +713,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="9">
-        <v>256</v>
+        <v>1948</v>
       </c>
       <c r="C3" s="9">
         <v>2</v>
@@ -731,7 +732,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="9">
-        <v>1438</v>
+        <v>2355</v>
       </c>
       <c r="C4" s="9">
         <v>2</v>
@@ -750,7 +751,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="9">
-        <v>510</v>
+        <v>358</v>
       </c>
       <c r="C5" s="9">
         <v>2</v>
@@ -769,7 +770,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="9">
-        <v>2100</v>
+        <v>408</v>
       </c>
       <c r="C6" s="9">
         <v>2</v>
@@ -788,7 +789,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="9">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="C7" s="9">
         <v>2</v>
@@ -807,10 +808,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="9">
-        <v>358</v>
+        <v>104</v>
       </c>
       <c r="C8" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
@@ -826,7 +827,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="9">
-        <v>408</v>
+        <v>256</v>
       </c>
       <c r="C9" s="9">
         <v>2</v>
@@ -845,7 +846,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="9">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="C10" s="9">
         <v>2</v>
@@ -864,10 +865,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="9">
-        <v>104</v>
+        <v>460</v>
       </c>
       <c r="C11" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -883,7 +884,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="9">
-        <v>256</v>
+        <v>204</v>
       </c>
       <c r="C12" s="9">
         <v>2</v>
@@ -902,7 +903,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="9">
-        <v>140</v>
+        <v>1020</v>
       </c>
       <c r="C13" s="9">
         <v>2</v>
@@ -921,7 +922,7 @@
         <v>15</v>
       </c>
       <c r="B14" s="9">
-        <v>460</v>
+        <v>256</v>
       </c>
       <c r="C14" s="9">
         <v>2</v>
@@ -940,7 +941,7 @@
         <v>16</v>
       </c>
       <c r="B15" s="9">
-        <v>204</v>
+        <v>306</v>
       </c>
       <c r="C15" s="9">
         <v>2</v>
@@ -959,7 +960,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="9">
-        <v>1020</v>
+        <v>10</v>
       </c>
       <c r="C16" s="9">
         <v>2</v>
@@ -978,7 +979,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="9">
-        <v>256</v>
+        <v>714</v>
       </c>
       <c r="C17" s="9">
         <v>2</v>
@@ -997,7 +998,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="9">
-        <v>306</v>
+        <v>16</v>
       </c>
       <c r="C18" s="9">
         <v>2</v>
@@ -1016,7 +1017,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="9">
-        <v>10</v>
+        <v>510</v>
       </c>
       <c r="C19" s="9">
         <v>2</v>
@@ -1030,81 +1031,24 @@
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="9">
-        <v>714</v>
-      </c>
-      <c r="C20" s="9">
-        <v>2</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="9">
-        <v>16</v>
-      </c>
-      <c r="C21" s="9">
-        <v>2</v>
-      </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="9">
-        <v>510</v>
-      </c>
-      <c r="C22" s="9">
-        <v>2</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-    </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="12">
+      <c r="B20" s="12">
         <v>204</v>
       </c>
-      <c r="C23" s="12">
-        <v>2</v>
-      </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
+      <c r="C20" s="12">
+        <v>2</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
building depth done and added comments and factored
</commit_message>
<xml_diff>
--- a/data/relationships/agent_size.xlsx
+++ b/data/relationships/agent_size.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanda\Work\spatial_computing\data\relationships\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CD3851-B043-4D1C-9C44-81835FCEED95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78E0351-FFBC-4C9C-BA36-9867BCE0FD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -655,7 +655,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -718,7 +718,9 @@
       <c r="C3" s="9">
         <v>2</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="5">
+        <v>13</v>
+      </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -737,7 +739,9 @@
       <c r="C4" s="9">
         <v>2</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="5">
+        <v>13</v>
+      </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
@@ -756,7 +760,9 @@
       <c r="C5" s="9">
         <v>2</v>
       </c>
-      <c r="D5" s="8"/>
+      <c r="D5" s="5">
+        <v>13</v>
+      </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
@@ -775,7 +781,9 @@
       <c r="C6" s="9">
         <v>2</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="5">
+        <v>13</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -794,7 +802,9 @@
       <c r="C7" s="9">
         <v>2</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="5">
+        <v>13</v>
+      </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -813,7 +823,9 @@
       <c r="C8" s="9">
         <v>4</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="5">
+        <v>13</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -832,7 +844,9 @@
       <c r="C9" s="9">
         <v>2</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="5">
+        <v>13</v>
+      </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
@@ -851,7 +865,9 @@
       <c r="C10" s="9">
         <v>2</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="5">
+        <v>13</v>
+      </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
@@ -870,7 +886,9 @@
       <c r="C11" s="9">
         <v>2</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="5">
+        <v>13</v>
+      </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
@@ -889,7 +907,9 @@
       <c r="C12" s="9">
         <v>2</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="5">
+        <v>13</v>
+      </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
@@ -908,7 +928,9 @@
       <c r="C13" s="9">
         <v>2</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="5">
+        <v>13</v>
+      </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -927,7 +949,9 @@
       <c r="C14" s="9">
         <v>2</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="5">
+        <v>13</v>
+      </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
@@ -946,7 +970,9 @@
       <c r="C15" s="9">
         <v>2</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="5">
+        <v>13</v>
+      </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
@@ -965,7 +991,9 @@
       <c r="C16" s="9">
         <v>2</v>
       </c>
-      <c r="D16" s="8"/>
+      <c r="D16" s="5">
+        <v>13</v>
+      </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
@@ -984,7 +1012,9 @@
       <c r="C17" s="9">
         <v>2</v>
       </c>
-      <c r="D17" s="8"/>
+      <c r="D17" s="5">
+        <v>13</v>
+      </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
@@ -1003,7 +1033,9 @@
       <c r="C18" s="9">
         <v>2</v>
       </c>
-      <c r="D18" s="8"/>
+      <c r="D18" s="5">
+        <v>13</v>
+      </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
@@ -1022,7 +1054,9 @@
       <c r="C19" s="9">
         <v>2</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" s="5">
+        <v>13</v>
+      </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
@@ -1041,7 +1075,9 @@
       <c r="C20" s="12">
         <v>2</v>
       </c>
-      <c r="D20" s="11"/>
+      <c r="D20" s="5">
+        <v>13</v>
+      </c>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>

</xml_diff>

<commit_message>
the growth process was run
</commit_message>
<xml_diff>
--- a/data/relationships/agent_size.xlsx
+++ b/data/relationships/agent_size.xlsx
@@ -5,20 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanda\Work\spatial_computing\data\relationships\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cobyb\Desktop\Desktop icons\Minor Spatial Computing\Github Tan\spatial_computing\data\relationships\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78E0351-FFBC-4C9C-BA36-9867BCE0FD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737D09C3-BC2B-4FF3-8F71-22AC7CCBC4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -655,7 +664,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -692,13 +701,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="6">
-        <v>1879</v>
+        <v>408</v>
       </c>
       <c r="C2" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -713,13 +722,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="9">
-        <v>1948</v>
+        <v>360</v>
       </c>
       <c r="C3" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -734,13 +743,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="9">
-        <v>2355</v>
+        <v>1530</v>
       </c>
       <c r="C4" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -755,13 +764,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="9">
-        <v>358</v>
+        <v>90</v>
       </c>
       <c r="C5" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
@@ -776,13 +785,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="9">
-        <v>408</v>
+        <v>102</v>
       </c>
       <c r="C6" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -797,13 +806,13 @@
         <v>8</v>
       </c>
       <c r="B7" s="9">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="C7" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -818,13 +827,13 @@
         <v>9</v>
       </c>
       <c r="B8" s="9">
-        <v>104</v>
+        <v>24</v>
       </c>
       <c r="C8" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D8" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -839,13 +848,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="9">
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="C9" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -860,13 +869,13 @@
         <v>11</v>
       </c>
       <c r="B10" s="9">
-        <v>140</v>
+        <v>36</v>
       </c>
       <c r="C10" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -881,13 +890,13 @@
         <v>12</v>
       </c>
       <c r="B11" s="9">
-        <v>460</v>
+        <v>114</v>
       </c>
       <c r="C11" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -902,13 +911,13 @@
         <v>13</v>
       </c>
       <c r="B12" s="9">
-        <v>204</v>
+        <v>52</v>
       </c>
       <c r="C12" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -923,13 +932,13 @@
         <v>14</v>
       </c>
       <c r="B13" s="9">
-        <v>1020</v>
+        <v>256</v>
       </c>
       <c r="C13" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -944,13 +953,13 @@
         <v>15</v>
       </c>
       <c r="B14" s="9">
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="C14" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -965,13 +974,13 @@
         <v>16</v>
       </c>
       <c r="B15" s="9">
-        <v>306</v>
+        <v>76</v>
       </c>
       <c r="C15" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -986,13 +995,13 @@
         <v>17</v>
       </c>
       <c r="B16" s="9">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C16" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1007,13 +1016,13 @@
         <v>18</v>
       </c>
       <c r="B17" s="9">
-        <v>714</v>
+        <v>178</v>
       </c>
       <c r="C17" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1028,13 +1037,13 @@
         <v>19</v>
       </c>
       <c r="B18" s="9">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C18" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1049,13 +1058,13 @@
         <v>20</v>
       </c>
       <c r="B19" s="9">
-        <v>510</v>
+        <v>128</v>
       </c>
       <c r="C19" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1070,13 +1079,13 @@
         <v>21</v>
       </c>
       <c r="B20" s="12">
-        <v>204</v>
+        <v>52</v>
       </c>
       <c r="C20" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>

</xml_diff>

<commit_message>
updated the voxel size and added distance fields for specific agents
</commit_message>
<xml_diff>
--- a/data/relationships/agent_size.xlsx
+++ b/data/relationships/agent_size.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cobyb\Desktop\Desktop icons\Minor Spatial Computing\Github Tan\spatial_computing\data\relationships\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737D09C3-BC2B-4FF3-8F71-22AC7CCBC4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90D8CD8-8518-410E-A14E-0BB8AFC968D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8508" yWindow="-300" windowWidth="12960" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -663,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,13 +701,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="6">
-        <v>408</v>
+        <v>91</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
       </c>
       <c r="D2" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -722,13 +722,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="9">
-        <v>360</v>
+        <v>80</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
       </c>
       <c r="D3" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -743,13 +743,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="9">
-        <v>1530</v>
+        <v>340</v>
       </c>
       <c r="C4" s="9">
         <v>1</v>
       </c>
       <c r="D4" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -764,13 +764,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="9">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="C5" s="9">
         <v>1</v>
       </c>
       <c r="D5" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
@@ -785,13 +785,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="9">
-        <v>102</v>
+        <v>23</v>
       </c>
       <c r="C6" s="9">
         <v>1</v>
       </c>
       <c r="D6" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -806,13 +806,13 @@
         <v>8</v>
       </c>
       <c r="B7" s="9">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C7" s="9">
         <v>1</v>
       </c>
       <c r="D7" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -827,13 +827,13 @@
         <v>9</v>
       </c>
       <c r="B8" s="9">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C8" s="9">
         <v>1</v>
       </c>
       <c r="D8" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -848,13 +848,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="9">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="C9" s="9">
         <v>1</v>
       </c>
       <c r="D9" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -869,13 +869,13 @@
         <v>11</v>
       </c>
       <c r="B10" s="9">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C10" s="9">
         <v>1</v>
       </c>
       <c r="D10" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -890,13 +890,13 @@
         <v>12</v>
       </c>
       <c r="B11" s="9">
-        <v>114</v>
+        <v>26</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
       </c>
       <c r="D11" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -911,13 +911,13 @@
         <v>13</v>
       </c>
       <c r="B12" s="9">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="C12" s="9">
         <v>1</v>
       </c>
       <c r="D12" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -932,13 +932,13 @@
         <v>14</v>
       </c>
       <c r="B13" s="9">
-        <v>256</v>
+        <v>57</v>
       </c>
       <c r="C13" s="9">
         <v>1</v>
       </c>
       <c r="D13" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -953,13 +953,13 @@
         <v>15</v>
       </c>
       <c r="B14" s="9">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="C14" s="9">
         <v>1</v>
       </c>
       <c r="D14" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -974,13 +974,13 @@
         <v>16</v>
       </c>
       <c r="B15" s="9">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="C15" s="9">
         <v>1</v>
       </c>
       <c r="D15" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -995,13 +995,13 @@
         <v>17</v>
       </c>
       <c r="B16" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="9">
         <v>1</v>
       </c>
       <c r="D16" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1016,13 +1016,13 @@
         <v>18</v>
       </c>
       <c r="B17" s="9">
-        <v>178</v>
+        <v>40</v>
       </c>
       <c r="C17" s="9">
         <v>1</v>
       </c>
       <c r="D17" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1037,13 +1037,13 @@
         <v>19</v>
       </c>
       <c r="B18" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C18" s="9">
         <v>1</v>
       </c>
       <c r="D18" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1058,13 +1058,13 @@
         <v>20</v>
       </c>
       <c r="B19" s="9">
-        <v>128</v>
+        <v>28</v>
       </c>
       <c r="C19" s="9">
         <v>1</v>
       </c>
       <c r="D19" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1079,13 +1079,13 @@
         <v>21</v>
       </c>
       <c r="B20" s="12">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="C20" s="12">
         <v>1</v>
       </c>
       <c r="D20" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>

</xml_diff>

<commit_message>
200 frames were ran on the growth
</commit_message>
<xml_diff>
--- a/data/relationships/agent_size.xlsx
+++ b/data/relationships/agent_size.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cobyb\Desktop\Desktop icons\Minor Spatial Computing\Github Tan\spatial_computing\data\relationships\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90D8CD8-8518-410E-A14E-0BB8AFC968D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3160B6-2B9E-4E4E-BA14-343469F43217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8508" yWindow="-300" windowWidth="12960" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -664,7 +664,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>